<commit_message>
added function to create csv file and folder
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/beamafilm/beamafilm.xlsx
+++ b/tests/testthat/testdata/beamafilm/beamafilm.xlsx
@@ -418,7 +418,7 @@
         </is>
       </c>
       <c r="E2">
-        <v>13835</v>
+        <v>18946</v>
       </c>
       <c r="F2" s="2">
         <v>44255</v>
@@ -446,7 +446,7 @@
         </is>
       </c>
       <c r="E3">
-        <v>17923</v>
+        <v>5304</v>
       </c>
       <c r="F3" s="2">
         <v>44255</v>
@@ -474,7 +474,7 @@
         </is>
       </c>
       <c r="E4">
-        <v>1936</v>
+        <v>18016</v>
       </c>
       <c r="F4" s="2">
         <v>44255</v>
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="E5">
-        <v>8830</v>
+        <v>1666</v>
       </c>
       <c r="F5" s="2">
         <v>44255</v>
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="E6">
-        <v>5018</v>
+        <v>16533</v>
       </c>
       <c r="F6" s="2">
         <v>44255</v>
@@ -558,7 +558,7 @@
         </is>
       </c>
       <c r="E7">
-        <v>7656</v>
+        <v>3102</v>
       </c>
       <c r="F7" s="2">
         <v>44255</v>
@@ -586,7 +586,7 @@
         </is>
       </c>
       <c r="E8">
-        <v>17052</v>
+        <v>6841</v>
       </c>
       <c r="F8" s="2">
         <v>44255</v>
@@ -614,7 +614,7 @@
         </is>
       </c>
       <c r="E9">
-        <v>16413</v>
+        <v>1146</v>
       </c>
       <c r="F9" s="2">
         <v>44255</v>
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="E10">
-        <v>19471</v>
+        <v>16797</v>
       </c>
       <c r="F10" s="2">
         <v>44255</v>
@@ -670,7 +670,7 @@
         </is>
       </c>
       <c r="E11">
-        <v>2175</v>
+        <v>15214</v>
       </c>
       <c r="F11" s="2">
         <v>44255</v>
@@ -698,7 +698,7 @@
         </is>
       </c>
       <c r="E12">
-        <v>13596</v>
+        <v>14293</v>
       </c>
       <c r="F12" s="2">
         <v>44255</v>
@@ -726,7 +726,7 @@
         </is>
       </c>
       <c r="E13">
-        <v>15689</v>
+        <v>12708</v>
       </c>
       <c r="F13" s="2">
         <v>44255</v>

</xml_diff>

<commit_message>
updated read file function, made get file name function, updated prepare beamafilm function
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/beamafilm/beamafilm.xlsx
+++ b/tests/testthat/testdata/beamafilm/beamafilm.xlsx
@@ -418,7 +418,7 @@
         </is>
       </c>
       <c r="E2">
-        <v>18946</v>
+        <v>18561</v>
       </c>
       <c r="F2" s="2">
         <v>44255</v>
@@ -446,7 +446,7 @@
         </is>
       </c>
       <c r="E3">
-        <v>5304</v>
+        <v>15392</v>
       </c>
       <c r="F3" s="2">
         <v>44255</v>
@@ -474,7 +474,7 @@
         </is>
       </c>
       <c r="E4">
-        <v>18016</v>
+        <v>7834</v>
       </c>
       <c r="F4" s="2">
         <v>44255</v>
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="E5">
-        <v>1666</v>
+        <v>13540</v>
       </c>
       <c r="F5" s="2">
         <v>44255</v>
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="E6">
-        <v>16533</v>
+        <v>18132</v>
       </c>
       <c r="F6" s="2">
         <v>44255</v>
@@ -558,7 +558,7 @@
         </is>
       </c>
       <c r="E7">
-        <v>3102</v>
+        <v>4648</v>
       </c>
       <c r="F7" s="2">
         <v>44255</v>
@@ -586,7 +586,7 @@
         </is>
       </c>
       <c r="E8">
-        <v>6841</v>
+        <v>13210</v>
       </c>
       <c r="F8" s="2">
         <v>44255</v>
@@ -614,7 +614,7 @@
         </is>
       </c>
       <c r="E9">
-        <v>1146</v>
+        <v>11792</v>
       </c>
       <c r="F9" s="2">
         <v>44255</v>
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="E10">
-        <v>16797</v>
+        <v>6013</v>
       </c>
       <c r="F10" s="2">
         <v>44255</v>
@@ -670,7 +670,7 @@
         </is>
       </c>
       <c r="E11">
-        <v>15214</v>
+        <v>16243</v>
       </c>
       <c r="F11" s="2">
         <v>44255</v>
@@ -698,7 +698,7 @@
         </is>
       </c>
       <c r="E12">
-        <v>14293</v>
+        <v>2275</v>
       </c>
       <c r="F12" s="2">
         <v>44255</v>
@@ -726,7 +726,7 @@
         </is>
       </c>
       <c r="E13">
-        <v>12708</v>
+        <v>1979</v>
       </c>
       <c r="F13" s="2">
         <v>44255</v>

</xml_diff>

<commit_message>
refactored file_format to file_type
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/beamafilm/beamafilm.xlsx
+++ b/tests/testthat/testdata/beamafilm/beamafilm.xlsx
@@ -418,7 +418,7 @@
         </is>
       </c>
       <c r="E2">
-        <v>18561</v>
+        <v>9881</v>
       </c>
       <c r="F2" s="2">
         <v>44255</v>
@@ -446,7 +446,7 @@
         </is>
       </c>
       <c r="E3">
-        <v>15392</v>
+        <v>2343</v>
       </c>
       <c r="F3" s="2">
         <v>44255</v>
@@ -474,7 +474,7 @@
         </is>
       </c>
       <c r="E4">
-        <v>7834</v>
+        <v>10950</v>
       </c>
       <c r="F4" s="2">
         <v>44255</v>
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="E5">
-        <v>13540</v>
+        <v>2697</v>
       </c>
       <c r="F5" s="2">
         <v>44255</v>
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="E6">
-        <v>18132</v>
+        <v>19513</v>
       </c>
       <c r="F6" s="2">
         <v>44255</v>
@@ -558,7 +558,7 @@
         </is>
       </c>
       <c r="E7">
-        <v>4648</v>
+        <v>3655</v>
       </c>
       <c r="F7" s="2">
         <v>44255</v>
@@ -586,7 +586,7 @@
         </is>
       </c>
       <c r="E8">
-        <v>13210</v>
+        <v>1128</v>
       </c>
       <c r="F8" s="2">
         <v>44255</v>
@@ -614,7 +614,7 @@
         </is>
       </c>
       <c r="E9">
-        <v>11792</v>
+        <v>5248</v>
       </c>
       <c r="F9" s="2">
         <v>44255</v>
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="E10">
-        <v>6013</v>
+        <v>14597</v>
       </c>
       <c r="F10" s="2">
         <v>44255</v>
@@ -670,7 +670,7 @@
         </is>
       </c>
       <c r="E11">
-        <v>16243</v>
+        <v>13065</v>
       </c>
       <c r="F11" s="2">
         <v>44255</v>
@@ -698,7 +698,7 @@
         </is>
       </c>
       <c r="E12">
-        <v>2275</v>
+        <v>16663</v>
       </c>
       <c r="F12" s="2">
         <v>44255</v>
@@ -726,7 +726,7 @@
         </is>
       </c>
       <c r="E13">
-        <v>1979</v>
+        <v>11807</v>
       </c>
       <c r="F13" s="2">
         <v>44255</v>

</xml_diff>

<commit_message>
fixed read file function
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/beamafilm/beamafilm.xlsx
+++ b/tests/testthat/testdata/beamafilm/beamafilm.xlsx
@@ -418,7 +418,7 @@
         </is>
       </c>
       <c r="E2">
-        <v>9881</v>
+        <v>9560</v>
       </c>
       <c r="F2" s="2">
         <v>44255</v>
@@ -446,7 +446,7 @@
         </is>
       </c>
       <c r="E3">
-        <v>2343</v>
+        <v>15930</v>
       </c>
       <c r="F3" s="2">
         <v>44255</v>
@@ -474,7 +474,7 @@
         </is>
       </c>
       <c r="E4">
-        <v>10950</v>
+        <v>7689</v>
       </c>
       <c r="F4" s="2">
         <v>44255</v>
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="E5">
-        <v>2697</v>
+        <v>4755</v>
       </c>
       <c r="F5" s="2">
         <v>44255</v>
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="E6">
-        <v>19513</v>
+        <v>17670</v>
       </c>
       <c r="F6" s="2">
         <v>44255</v>
@@ -558,7 +558,7 @@
         </is>
       </c>
       <c r="E7">
-        <v>3655</v>
+        <v>13068</v>
       </c>
       <c r="F7" s="2">
         <v>44255</v>
@@ -586,7 +586,7 @@
         </is>
       </c>
       <c r="E8">
-        <v>1128</v>
+        <v>12517</v>
       </c>
       <c r="F8" s="2">
         <v>44255</v>
@@ -614,7 +614,7 @@
         </is>
       </c>
       <c r="E9">
-        <v>5248</v>
+        <v>3154</v>
       </c>
       <c r="F9" s="2">
         <v>44255</v>
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="E10">
-        <v>14597</v>
+        <v>13002</v>
       </c>
       <c r="F10" s="2">
         <v>44255</v>
@@ -670,7 +670,7 @@
         </is>
       </c>
       <c r="E11">
-        <v>13065</v>
+        <v>12217</v>
       </c>
       <c r="F11" s="2">
         <v>44255</v>
@@ -698,7 +698,7 @@
         </is>
       </c>
       <c r="E12">
-        <v>16663</v>
+        <v>10818</v>
       </c>
       <c r="F12" s="2">
         <v>44255</v>
@@ -726,7 +726,7 @@
         </is>
       </c>
       <c r="E13">
-        <v>11807</v>
+        <v>1894</v>
       </c>
       <c r="F13" s="2">
         <v>44255</v>

</xml_diff>

<commit_message>
updated read file function to handle row skipping and reading in file names
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/beamafilm/beamafilm.xlsx
+++ b/tests/testthat/testdata/beamafilm/beamafilm.xlsx
@@ -418,7 +418,7 @@
         </is>
       </c>
       <c r="E2">
-        <v>6064</v>
+        <v>10949</v>
       </c>
       <c r="F2" s="2">
         <v>44255</v>
@@ -446,7 +446,7 @@
         </is>
       </c>
       <c r="E3">
-        <v>9713</v>
+        <v>13470</v>
       </c>
       <c r="F3" s="2">
         <v>44255</v>
@@ -474,7 +474,7 @@
         </is>
       </c>
       <c r="E4">
-        <v>18505</v>
+        <v>13939</v>
       </c>
       <c r="F4" s="2">
         <v>44255</v>
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="E5">
-        <v>12409</v>
+        <v>10560</v>
       </c>
       <c r="F5" s="2">
         <v>44255</v>
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="E6">
-        <v>7456</v>
+        <v>12942</v>
       </c>
       <c r="F6" s="2">
         <v>44255</v>
@@ -558,7 +558,7 @@
         </is>
       </c>
       <c r="E7">
-        <v>2375</v>
+        <v>17625</v>
       </c>
       <c r="F7" s="2">
         <v>44255</v>
@@ -586,7 +586,7 @@
         </is>
       </c>
       <c r="E8">
-        <v>3183</v>
+        <v>5050</v>
       </c>
       <c r="F8" s="2">
         <v>44255</v>
@@ -614,7 +614,7 @@
         </is>
       </c>
       <c r="E9">
-        <v>5877</v>
+        <v>14611</v>
       </c>
       <c r="F9" s="2">
         <v>44255</v>
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="E10">
-        <v>4806</v>
+        <v>15741</v>
       </c>
       <c r="F10" s="2">
         <v>44255</v>
@@ -670,7 +670,7 @@
         </is>
       </c>
       <c r="E11">
-        <v>5033</v>
+        <v>10299</v>
       </c>
       <c r="F11" s="2">
         <v>44255</v>
@@ -698,7 +698,7 @@
         </is>
       </c>
       <c r="E12">
-        <v>2692</v>
+        <v>17130</v>
       </c>
       <c r="F12" s="2">
         <v>44255</v>
@@ -726,7 +726,7 @@
         </is>
       </c>
       <c r="E13">
-        <v>9766</v>
+        <v>18324</v>
       </c>
       <c r="F13" s="2">
         <v>44255</v>

</xml_diff>

<commit_message>
added unit test for discovery
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/beamafilm/beamafilm.xlsx
+++ b/tests/testthat/testdata/beamafilm/beamafilm.xlsx
@@ -418,7 +418,7 @@
         </is>
       </c>
       <c r="E2">
-        <v>10949</v>
+        <v>5764</v>
       </c>
       <c r="F2" s="2">
         <v>44255</v>
@@ -446,7 +446,7 @@
         </is>
       </c>
       <c r="E3">
-        <v>13470</v>
+        <v>6330</v>
       </c>
       <c r="F3" s="2">
         <v>44255</v>
@@ -474,7 +474,7 @@
         </is>
       </c>
       <c r="E4">
-        <v>13939</v>
+        <v>3300</v>
       </c>
       <c r="F4" s="2">
         <v>44255</v>
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="E5">
-        <v>10560</v>
+        <v>18174</v>
       </c>
       <c r="F5" s="2">
         <v>44255</v>
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="E6">
-        <v>12942</v>
+        <v>15489</v>
       </c>
       <c r="F6" s="2">
         <v>44255</v>
@@ -558,7 +558,7 @@
         </is>
       </c>
       <c r="E7">
-        <v>17625</v>
+        <v>1406</v>
       </c>
       <c r="F7" s="2">
         <v>44255</v>
@@ -586,7 +586,7 @@
         </is>
       </c>
       <c r="E8">
-        <v>5050</v>
+        <v>4296</v>
       </c>
       <c r="F8" s="2">
         <v>44255</v>
@@ -614,7 +614,7 @@
         </is>
       </c>
       <c r="E9">
-        <v>14611</v>
+        <v>8026</v>
       </c>
       <c r="F9" s="2">
         <v>44255</v>
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="E10">
-        <v>15741</v>
+        <v>3274</v>
       </c>
       <c r="F10" s="2">
         <v>44255</v>
@@ -670,7 +670,7 @@
         </is>
       </c>
       <c r="E11">
-        <v>10299</v>
+        <v>18319</v>
       </c>
       <c r="F11" s="2">
         <v>44255</v>
@@ -698,7 +698,7 @@
         </is>
       </c>
       <c r="E12">
-        <v>17130</v>
+        <v>13587</v>
       </c>
       <c r="F12" s="2">
         <v>44255</v>
@@ -726,7 +726,7 @@
         </is>
       </c>
       <c r="E13">
-        <v>18324</v>
+        <v>9147</v>
       </c>
       <c r="F13" s="2">
         <v>44255</v>

</xml_diff>

<commit_message>
removed warning from dir.create
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/beamafilm/beamafilm.xlsx
+++ b/tests/testthat/testdata/beamafilm/beamafilm.xlsx
@@ -418,7 +418,7 @@
         </is>
       </c>
       <c r="E2">
-        <v>5764</v>
+        <v>18474</v>
       </c>
       <c r="F2" s="2">
         <v>44255</v>
@@ -446,7 +446,7 @@
         </is>
       </c>
       <c r="E3">
-        <v>6330</v>
+        <v>1713</v>
       </c>
       <c r="F3" s="2">
         <v>44255</v>
@@ -474,7 +474,7 @@
         </is>
       </c>
       <c r="E4">
-        <v>3300</v>
+        <v>11700</v>
       </c>
       <c r="F4" s="2">
         <v>44255</v>
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="E5">
-        <v>18174</v>
+        <v>17902</v>
       </c>
       <c r="F5" s="2">
         <v>44255</v>
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="E6">
-        <v>15489</v>
+        <v>15421</v>
       </c>
       <c r="F6" s="2">
         <v>44255</v>
@@ -558,7 +558,7 @@
         </is>
       </c>
       <c r="E7">
-        <v>1406</v>
+        <v>1483</v>
       </c>
       <c r="F7" s="2">
         <v>44255</v>
@@ -586,7 +586,7 @@
         </is>
       </c>
       <c r="E8">
-        <v>4296</v>
+        <v>5235</v>
       </c>
       <c r="F8" s="2">
         <v>44255</v>
@@ -614,7 +614,7 @@
         </is>
       </c>
       <c r="E9">
-        <v>8026</v>
+        <v>13898</v>
       </c>
       <c r="F9" s="2">
         <v>44255</v>
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="E10">
-        <v>3274</v>
+        <v>19552</v>
       </c>
       <c r="F10" s="2">
         <v>44255</v>
@@ -670,7 +670,7 @@
         </is>
       </c>
       <c r="E11">
-        <v>18319</v>
+        <v>5269</v>
       </c>
       <c r="F11" s="2">
         <v>44255</v>
@@ -698,7 +698,7 @@
         </is>
       </c>
       <c r="E12">
-        <v>13587</v>
+        <v>17354</v>
       </c>
       <c r="F12" s="2">
         <v>44255</v>
@@ -726,7 +726,7 @@
         </is>
       </c>
       <c r="E13">
-        <v>9147</v>
+        <v>5648</v>
       </c>
       <c r="F13" s="2">
         <v>44255</v>

</xml_diff>

<commit_message>
added @export to write file function
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/beamafilm/beamafilm.xlsx
+++ b/tests/testthat/testdata/beamafilm/beamafilm.xlsx
@@ -418,7 +418,7 @@
         </is>
       </c>
       <c r="E2">
-        <v>18474</v>
+        <v>5252</v>
       </c>
       <c r="F2" s="2">
         <v>44255</v>
@@ -446,7 +446,7 @@
         </is>
       </c>
       <c r="E3">
-        <v>1713</v>
+        <v>6395</v>
       </c>
       <c r="F3" s="2">
         <v>44255</v>
@@ -474,7 +474,7 @@
         </is>
       </c>
       <c r="E4">
-        <v>11700</v>
+        <v>8107</v>
       </c>
       <c r="F4" s="2">
         <v>44255</v>
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="E5">
-        <v>17902</v>
+        <v>3718</v>
       </c>
       <c r="F5" s="2">
         <v>44255</v>
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="E6">
-        <v>15421</v>
+        <v>6009</v>
       </c>
       <c r="F6" s="2">
         <v>44255</v>
@@ -558,7 +558,7 @@
         </is>
       </c>
       <c r="E7">
-        <v>1483</v>
+        <v>13877</v>
       </c>
       <c r="F7" s="2">
         <v>44255</v>
@@ -586,7 +586,7 @@
         </is>
       </c>
       <c r="E8">
-        <v>5235</v>
+        <v>15603</v>
       </c>
       <c r="F8" s="2">
         <v>44255</v>
@@ -614,7 +614,7 @@
         </is>
       </c>
       <c r="E9">
-        <v>13898</v>
+        <v>11396</v>
       </c>
       <c r="F9" s="2">
         <v>44255</v>
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="E10">
-        <v>19552</v>
+        <v>19883</v>
       </c>
       <c r="F10" s="2">
         <v>44255</v>
@@ -670,7 +670,7 @@
         </is>
       </c>
       <c r="E11">
-        <v>5269</v>
+        <v>6974</v>
       </c>
       <c r="F11" s="2">
         <v>44255</v>
@@ -698,7 +698,7 @@
         </is>
       </c>
       <c r="E12">
-        <v>17354</v>
+        <v>19523</v>
       </c>
       <c r="F12" s="2">
         <v>44255</v>
@@ -726,7 +726,7 @@
         </is>
       </c>
       <c r="E13">
-        <v>5648</v>
+        <v>8218</v>
       </c>
       <c r="F13" s="2">
         <v>44255</v>

</xml_diff>

<commit_message>
added @export to most functions
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/beamafilm/beamafilm.xlsx
+++ b/tests/testthat/testdata/beamafilm/beamafilm.xlsx
@@ -418,7 +418,7 @@
         </is>
       </c>
       <c r="E2">
-        <v>5252</v>
+        <v>4825</v>
       </c>
       <c r="F2" s="2">
         <v>44255</v>
@@ -446,7 +446,7 @@
         </is>
       </c>
       <c r="E3">
-        <v>6395</v>
+        <v>16877</v>
       </c>
       <c r="F3" s="2">
         <v>44255</v>
@@ -474,7 +474,7 @@
         </is>
       </c>
       <c r="E4">
-        <v>8107</v>
+        <v>15186</v>
       </c>
       <c r="F4" s="2">
         <v>44255</v>
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="E5">
-        <v>3718</v>
+        <v>6872</v>
       </c>
       <c r="F5" s="2">
         <v>44255</v>
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="E6">
-        <v>6009</v>
+        <v>8510</v>
       </c>
       <c r="F6" s="2">
         <v>44255</v>
@@ -558,7 +558,7 @@
         </is>
       </c>
       <c r="E7">
-        <v>13877</v>
+        <v>12634</v>
       </c>
       <c r="F7" s="2">
         <v>44255</v>
@@ -586,7 +586,7 @@
         </is>
       </c>
       <c r="E8">
-        <v>15603</v>
+        <v>7311</v>
       </c>
       <c r="F8" s="2">
         <v>44255</v>
@@ -614,7 +614,7 @@
         </is>
       </c>
       <c r="E9">
-        <v>11396</v>
+        <v>1390</v>
       </c>
       <c r="F9" s="2">
         <v>44255</v>
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="E10">
-        <v>19883</v>
+        <v>15772</v>
       </c>
       <c r="F10" s="2">
         <v>44255</v>
@@ -670,7 +670,7 @@
         </is>
       </c>
       <c r="E11">
-        <v>6974</v>
+        <v>10721</v>
       </c>
       <c r="F11" s="2">
         <v>44255</v>
@@ -698,7 +698,7 @@
         </is>
       </c>
       <c r="E12">
-        <v>19523</v>
+        <v>11069</v>
       </c>
       <c r="F12" s="2">
         <v>44255</v>
@@ -726,7 +726,7 @@
         </is>
       </c>
       <c r="E13">
-        <v>8218</v>
+        <v>1295</v>
       </c>
       <c r="F13" s="2">
         <v>44255</v>

</xml_diff>

<commit_message>
updated read file function to accept file extension
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/beamafilm/beamafilm.xlsx
+++ b/tests/testthat/testdata/beamafilm/beamafilm.xlsx
@@ -418,7 +418,7 @@
         </is>
       </c>
       <c r="E2">
-        <v>4825</v>
+        <v>11955</v>
       </c>
       <c r="F2" s="2">
         <v>44255</v>
@@ -446,7 +446,7 @@
         </is>
       </c>
       <c r="E3">
-        <v>16877</v>
+        <v>4162</v>
       </c>
       <c r="F3" s="2">
         <v>44255</v>
@@ -474,7 +474,7 @@
         </is>
       </c>
       <c r="E4">
-        <v>15186</v>
+        <v>19405</v>
       </c>
       <c r="F4" s="2">
         <v>44255</v>
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="E5">
-        <v>6872</v>
+        <v>16325</v>
       </c>
       <c r="F5" s="2">
         <v>44255</v>
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="E6">
-        <v>8510</v>
+        <v>14305</v>
       </c>
       <c r="F6" s="2">
         <v>44255</v>
@@ -558,7 +558,7 @@
         </is>
       </c>
       <c r="E7">
-        <v>12634</v>
+        <v>7527</v>
       </c>
       <c r="F7" s="2">
         <v>44255</v>
@@ -586,7 +586,7 @@
         </is>
       </c>
       <c r="E8">
-        <v>7311</v>
+        <v>4440</v>
       </c>
       <c r="F8" s="2">
         <v>44255</v>
@@ -614,7 +614,7 @@
         </is>
       </c>
       <c r="E9">
-        <v>1390</v>
+        <v>9320</v>
       </c>
       <c r="F9" s="2">
         <v>44255</v>
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="E10">
-        <v>15772</v>
+        <v>12338</v>
       </c>
       <c r="F10" s="2">
         <v>44255</v>
@@ -670,7 +670,7 @@
         </is>
       </c>
       <c r="E11">
-        <v>10721</v>
+        <v>13609</v>
       </c>
       <c r="F11" s="2">
         <v>44255</v>
@@ -698,7 +698,7 @@
         </is>
       </c>
       <c r="E12">
-        <v>11069</v>
+        <v>12930</v>
       </c>
       <c r="F12" s="2">
         <v>44255</v>
@@ -726,7 +726,7 @@
         </is>
       </c>
       <c r="E13">
-        <v>1295</v>
+        <v>14420</v>
       </c>
       <c r="F13" s="2">
         <v>44255</v>

</xml_diff>